<commit_message>
added code for reading multiple sheets and rows from excel sheet
</commit_message>
<xml_diff>
--- a/excel/data.xlsx
+++ b/excel/data.xlsx
@@ -8,12 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/anupamadhir/workspace/SeleniumHRProject/excel/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{61FAC49A-903D-7C47-8FE5-22331146FA50}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A643BB22-AE50-D446-913B-2C58BBB9CF62}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1600" yWindow="600" windowWidth="28040" windowHeight="15940" xr2:uid="{75DE19C7-9349-604B-B4FA-2A9D5A2BE6CC}"/>
+    <workbookView xWindow="780" yWindow="460" windowWidth="28040" windowHeight="15940" activeTab="1" xr2:uid="{75DE19C7-9349-604B-B4FA-2A9D5A2BE6CC}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="AddLeave" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="181029"/>
   <extLst>
@@ -33,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="14">
   <si>
     <t>Username</t>
   </si>
@@ -45,14 +46,52 @@
   </si>
   <si>
     <t>admin123</t>
+  </si>
+  <si>
+    <t>Employee</t>
+  </si>
+  <si>
+    <t>Leave Type</t>
+  </si>
+  <si>
+    <t>Leave Period</t>
+  </si>
+  <si>
+    <t>Entitlement</t>
+  </si>
+  <si>
+    <t>Russel</t>
+  </si>
+  <si>
+    <t>2020-01-01$$2020-12-31</t>
+  </si>
+  <si>
+    <t>4</t>
+  </si>
+  <si>
+    <t>20</t>
+  </si>
+  <si>
+    <t>3</t>
+  </si>
+  <si>
+    <t>30</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
       <sz val="12"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -80,8 +119,10 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -398,7 +439,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A0697D74-9BCF-464C-9E24-E8112BA275C1}">
   <dimension ref="A1:B2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
@@ -423,4 +464,64 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{361FDEA2-F18E-154B-8B50-03064018DA32}">
+  <dimension ref="A1:D3"/>
+  <sheetViews>
+    <sheetView tabSelected="1" zoomScale="223" zoomScaleNormal="223" workbookViewId="0">
+      <selection activeCell="C6" sqref="C6"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="3" max="3" width="22.33203125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A2" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="D2" s="2" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A3" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="C3" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="D3" s="2" t="s">
+        <v>13</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>